<commit_message>
maj recup bdc début année
</commit_message>
<xml_diff>
--- a/test_xlsx_BDC.xlsx
+++ b/test_xlsx_BDC.xlsx
@@ -107,7 +107,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
@@ -166,114 +166,114 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="A2" s="0" t="n">
-        <v>80216</v>
+        <v>81401</v>
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>DN002XK</t>
+          <t>FG852BW</t>
         </is>
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>garage arrault</t>
+          <t>Antonin LAMPIN</t>
         </is>
       </c>
       <c r="D2" s="0" t="n">
-        <v>6900.00</v>
+        <v>12833.33</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>6900.00</v>
+        <v>15400.00</v>
       </c>
       <c r="F2" s="0" t="inlineStr">
         <is>
-          <t>CLEMENT SAUSSET </t>
+          <t>MOSSO MAMET </t>
         </is>
       </c>
       <c r="G2" s="0" t="inlineStr">
         <is>
-          <t>2023/06/14</t>
+          <t>2023/10/11</t>
         </is>
       </c>
       <c r="H2" s="0" t="inlineStr">
         <is>
-          <t>VENTE MARCHAND</t>
+          <t>VENTE PARTICULIER</t>
         </is>
       </c>
       <c r="I2" s="0" t="inlineStr">
         <is>
-          <t>VF7SCHMZ6FW520717</t>
+          <t>WF0NXXGCHNKE29395</t>
         </is>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="A3" s="0" t="n">
-        <v>80217</v>
+        <v>81402</v>
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
-          <t>FV841AV</t>
+          <t>FH391ZE</t>
         </is>
       </c>
       <c r="C3" s="0" t="inlineStr">
         <is>
-          <t>garage caillon</t>
+          <t>lena salle</t>
         </is>
       </c>
       <c r="D3" s="0" t="n">
-        <v>12083.33</v>
+        <v>9083.33</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>14500.00</v>
+        <v>10900.00</v>
       </c>
       <c r="F3" s="0" t="inlineStr">
         <is>
-          <t>CLEMENT SAUSSET </t>
+          <t>Patrice QUIET </t>
         </is>
       </c>
       <c r="G3" s="0" t="inlineStr">
         <is>
-          <t>2023/06/14</t>
+          <t>2023/10/11</t>
         </is>
       </c>
       <c r="H3" s="0" t="inlineStr">
         <is>
-          <t>VENTE MARCHAND</t>
+          <t>VENTE PARTICULIER</t>
         </is>
       </c>
       <c r="I3" s="0" t="inlineStr">
         <is>
-          <t>VF1RFE00166306583</t>
+          <t>VF1R9800163692898</t>
         </is>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="A4" s="0" t="n">
-        <v>80217</v>
+        <v>81403</v>
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
-          <t>FP610WT</t>
+          <t>GH410RB</t>
         </is>
       </c>
       <c r="C4" s="0" t="inlineStr">
         <is>
-          <t>garage caillon</t>
+          <t>UTILEO</t>
         </is>
       </c>
       <c r="D4" s="0" t="n">
-        <v>12000.00</v>
+        <v>29083.33</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>14400.00</v>
+        <v>34900.00</v>
       </c>
       <c r="F4" s="0" t="inlineStr">
         <is>
-          <t>CLEMENT SAUSSET </t>
+          <t>GUILLAUME HONNERT </t>
         </is>
       </c>
       <c r="G4" s="0" t="inlineStr">
         <is>
-          <t>2023/06/14</t>
+          <t>2023/10/11</t>
         </is>
       </c>
       <c r="H4" s="0" t="inlineStr">
@@ -283,38 +283,38 @@
       </c>
       <c r="I4" s="0" t="inlineStr">
         <is>
-          <t>VF1RFE00365061257</t>
+          <t>ZCFCE35BX0D711667</t>
         </is>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
       <c r="A5" s="0" t="n">
-        <v>80218</v>
+        <v>81403</v>
       </c>
       <c r="B5" s="0" t="inlineStr">
         <is>
-          <t>EG197DT</t>
+          <t>GH192RB</t>
         </is>
       </c>
       <c r="C5" s="0" t="inlineStr">
         <is>
-          <t>FCN</t>
+          <t>UTILEO</t>
         </is>
       </c>
       <c r="D5" s="0" t="n">
-        <v>18250.00</v>
+        <v>29083.33</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>21900.00</v>
+        <v>34900.00</v>
       </c>
       <c r="F5" s="0" t="inlineStr">
         <is>
-          <t>ABDELKADER OUDINA </t>
+          <t>GUILLAUME HONNERT </t>
         </is>
       </c>
       <c r="G5" s="0" t="inlineStr">
         <is>
-          <t>2023/06/14</t>
+          <t>2023/10/11</t>
         </is>
       </c>
       <c r="H5" s="0" t="inlineStr">
@@ -324,79 +324,79 @@
       </c>
       <c r="I5" s="0" t="inlineStr">
         <is>
-          <t>VF1JL000X55814399</t>
+          <t>ZCFCE35B30D711655</t>
         </is>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
       <c r="A6" s="0" t="n">
-        <v>80219</v>
+        <v>81403</v>
       </c>
       <c r="B6" s="0" t="inlineStr">
         <is>
-          <t>FD578DR</t>
+          <t>GH419RB</t>
         </is>
       </c>
       <c r="C6" s="0" t="inlineStr">
         <is>
-          <t>thibault dransard</t>
+          <t>UTILEO</t>
         </is>
       </c>
       <c r="D6" s="0" t="n">
-        <v>11396.26</v>
+        <v>29083.33</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>13628.76</v>
+        <v>34900.00</v>
       </c>
       <c r="F6" s="0" t="inlineStr">
         <is>
-          <t>Patrice QUIET </t>
+          <t>GUILLAUME HONNERT </t>
         </is>
       </c>
       <c r="G6" s="0" t="inlineStr">
         <is>
-          <t>2023/06/14</t>
+          <t>2023/10/11</t>
         </is>
       </c>
       <c r="H6" s="0" t="inlineStr">
         <is>
-          <t>VENTE PARTICULIER</t>
+          <t>VENTE MARCHAND</t>
         </is>
       </c>
       <c r="I6" s="0" t="inlineStr">
         <is>
-          <t>VF3CCHNPSJT085719</t>
+          <t>ZCFCE35B70D711674</t>
         </is>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
       <c r="A7" s="0" t="n">
-        <v>80220</v>
+        <v>81403</v>
       </c>
       <c r="B7" s="0" t="inlineStr">
         <is>
-          <t>EN201EM</t>
+          <t>GH785RB</t>
         </is>
       </c>
       <c r="C7" s="0" t="inlineStr">
         <is>
-          <t>JTA</t>
+          <t>UTILEO</t>
         </is>
       </c>
       <c r="D7" s="0" t="n">
-        <v>19916.67</v>
+        <v>29083.33</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>23900.00</v>
+        <v>34900.00</v>
       </c>
       <c r="F7" s="0" t="inlineStr">
         <is>
-          <t>HUMBERTO ALVES </t>
+          <t>GUILLAUME HONNERT </t>
         </is>
       </c>
       <c r="G7" s="0" t="inlineStr">
         <is>
-          <t>2023/06/14</t>
+          <t>2023/10/11</t>
         </is>
       </c>
       <c r="H7" s="0" t="inlineStr">
@@ -406,70 +406,70 @@
       </c>
       <c r="I7" s="0" t="inlineStr">
         <is>
-          <t>VF1JL000557856872</t>
+          <t>ZCFCE35BX0D711670</t>
         </is>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
       <c r="A8" s="0" t="n">
-        <v>80221</v>
+        <v>81403</v>
       </c>
       <c r="B8" s="0" t="inlineStr">
         <is>
-          <t>FL997YA</t>
+          <t>GH733RB</t>
         </is>
       </c>
       <c r="C8" s="0" t="inlineStr">
         <is>
-          <t>fiona de santi</t>
+          <t>UTILEO</t>
         </is>
       </c>
       <c r="D8" s="0" t="n">
-        <v>16453.5</v>
+        <v>29083.33</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>19686</v>
+        <v>34900.00</v>
       </c>
       <c r="F8" s="0" t="inlineStr">
         <is>
-          <t>CLEMENT SAUSSET </t>
+          <t>GUILLAUME HONNERT </t>
         </is>
       </c>
       <c r="G8" s="0" t="inlineStr">
         <is>
-          <t>2023/06/14</t>
+          <t>2023/10/11</t>
         </is>
       </c>
       <c r="H8" s="0" t="inlineStr">
         <is>
-          <t>VENTE PARTICULIER</t>
+          <t>VENTE MARCHAND</t>
         </is>
       </c>
       <c r="I8" s="0" t="inlineStr">
         <is>
-          <t>VF3MRHNSUKS466621</t>
+          <t>ZCFCE35B00D711659</t>
         </is>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
       <c r="A9" s="0" t="n">
-        <v>80222</v>
+        <v>81403</v>
       </c>
       <c r="B9" s="0" t="inlineStr">
         <is>
-          <t>FS280KT</t>
+          <t>GH802RB</t>
         </is>
       </c>
       <c r="C9" s="0" t="inlineStr">
         <is>
-          <t>SARL INTER VO FRANCE</t>
+          <t>UTILEO</t>
         </is>
       </c>
       <c r="D9" s="0" t="n">
-        <v>17900.00</v>
+        <v>31083.33</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>17900.00</v>
+        <v>37300.00</v>
       </c>
       <c r="F9" s="0" t="inlineStr">
         <is>
@@ -478,7 +478,7 @@
       </c>
       <c r="G9" s="0" t="inlineStr">
         <is>
-          <t>2023/06/14</t>
+          <t>2023/10/11</t>
         </is>
       </c>
       <c r="H9" s="0" t="inlineStr">
@@ -488,111 +488,111 @@
       </c>
       <c r="I9" s="0" t="inlineStr">
         <is>
-          <t>VR3UDYHYJLJ790745</t>
+          <t>ZCFCE35B605487713</t>
         </is>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
       <c r="A10" s="0" t="n">
-        <v>80223</v>
+        <v>81403</v>
       </c>
       <c r="B10" s="0" t="inlineStr">
         <is>
-          <t>FX860TE</t>
+          <t>GH593RB</t>
         </is>
       </c>
       <c r="C10" s="0" t="inlineStr">
         <is>
-          <t>KALATHOUNI RAFION ALI</t>
+          <t>UTILEO</t>
         </is>
       </c>
       <c r="D10" s="0" t="n">
-        <v>13975.26</v>
+        <v>31083.33</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>16707.76</v>
+        <v>37300.00</v>
       </c>
       <c r="F10" s="0" t="inlineStr">
         <is>
-          <t>TOM FERRAGU </t>
+          <t>GUILLAUME HONNERT </t>
         </is>
       </c>
       <c r="G10" s="0" t="inlineStr">
         <is>
-          <t>2023/06/14</t>
+          <t>2023/10/11</t>
         </is>
       </c>
       <c r="H10" s="0" t="inlineStr">
         <is>
-          <t>VENTE PARTICULIER</t>
+          <t>VENTE MARCHAND</t>
         </is>
       </c>
       <c r="I10" s="0" t="inlineStr">
         <is>
-          <t>VF1RFE00566453473</t>
+          <t>ZCFCE35B205489989</t>
         </is>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
       <c r="A11" s="0" t="n">
-        <v>80224</v>
+        <v>81404</v>
       </c>
       <c r="B11" s="0" t="inlineStr">
         <is>
-          <t>EQ888VS</t>
+          <t>FE023DZ</t>
         </is>
       </c>
       <c r="C11" s="0" t="inlineStr">
         <is>
-          <t>SANA OUNI</t>
+          <t>RS AUTO</t>
         </is>
       </c>
       <c r="D11" s="0" t="n">
-        <v>14557.26</v>
+        <v>3250.00</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>14639.76</v>
+        <v>3900.00</v>
       </c>
       <c r="F11" s="0" t="inlineStr">
         <is>
-          <t>MOSSO MAMET </t>
+          <t>YOHAN DUPONT </t>
         </is>
       </c>
       <c r="G11" s="0" t="inlineStr">
         <is>
-          <t>2023/06/14</t>
+          <t>2023/10/11</t>
         </is>
       </c>
       <c r="H11" s="0" t="inlineStr">
         <is>
-          <t>VENTE PARTICULIER</t>
+          <t>VENTE MARCHAND</t>
         </is>
       </c>
       <c r="I11" s="0" t="inlineStr">
         <is>
-          <t>VF1RFB00655526157</t>
+          <t>VF1R9800261012275</t>
         </is>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
       <c r="A12" s="0" t="n">
-        <v>80225</v>
+        <v>81405</v>
       </c>
       <c r="B12" s="0" t="inlineStr">
         <is>
-          <t>FP808PP</t>
+          <t>FY614LJ</t>
         </is>
       </c>
       <c r="C12" s="0" t="inlineStr">
         <is>
-          <t>ABDOULAYE SARR</t>
+          <t>Antonio Fernando ALVES DAS NEVES</t>
         </is>
       </c>
       <c r="D12" s="0" t="n">
-        <v>11453.26</v>
+        <v>14083.33</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>13685.76</v>
+        <v>16900.00</v>
       </c>
       <c r="F12" s="0" t="inlineStr">
         <is>
@@ -601,7 +601,7 @@
       </c>
       <c r="G12" s="0" t="inlineStr">
         <is>
-          <t>2023/06/14</t>
+          <t>2023/10/11</t>
         </is>
       </c>
       <c r="H12" s="0" t="inlineStr">
@@ -611,38 +611,38 @@
       </c>
       <c r="I12" s="0" t="inlineStr">
         <is>
-          <t>VF1RFB00065162125</t>
+          <t>WF02XXERK2MM87645</t>
         </is>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
       <c r="A13" s="0" t="n">
-        <v>80226</v>
+        <v>81406</v>
       </c>
       <c r="B13" s="0" t="inlineStr">
         <is>
-          <t>FT515VV</t>
+          <t>FQ957YL</t>
         </is>
       </c>
       <c r="C13" s="0" t="inlineStr">
         <is>
-          <t>GUILLAUME MAS AUTOMOBILES</t>
+          <t>AJC MOTORS</t>
         </is>
       </c>
       <c r="D13" s="0" t="n">
-        <v>11166.67</v>
+        <v>10416.67</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>13400.00</v>
+        <v>12500.00</v>
       </c>
       <c r="F13" s="0" t="inlineStr">
         <is>
-          <t>HUMBERTO ALVES </t>
+          <t>YOHAN DUPONT </t>
         </is>
       </c>
       <c r="G13" s="0" t="inlineStr">
         <is>
-          <t>2023/06/14</t>
+          <t>2023/10/11</t>
         </is>
       </c>
       <c r="H13" s="0" t="inlineStr">
@@ -652,202 +652,202 @@
       </c>
       <c r="I13" s="0" t="inlineStr">
         <is>
-          <t>VF1RFE00466232706</t>
+          <t>VF1RFB00765680216</t>
         </is>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
       <c r="A14" s="0" t="n">
-        <v>80227</v>
+        <v>81407</v>
       </c>
       <c r="B14" s="0" t="inlineStr">
         <is>
-          <t>FJ978NM</t>
+          <t>FR738LZ</t>
         </is>
       </c>
       <c r="C14" s="0" t="inlineStr">
         <is>
-          <t>DALLARD AUTOMBILES 64</t>
+          <t>Nabil MHIJAN</t>
         </is>
       </c>
       <c r="D14" s="0" t="n">
-        <v>9000.00</v>
+        <v>9916.67</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>9000.00</v>
+        <v>11900.00</v>
       </c>
       <c r="F14" s="0" t="inlineStr">
         <is>
-          <t>YOHAN DUPONT </t>
+          <t>MOSSO MAMET </t>
         </is>
       </c>
       <c r="G14" s="0" t="inlineStr">
         <is>
-          <t>2023/06/14</t>
+          <t>2023/10/11</t>
         </is>
       </c>
       <c r="H14" s="0" t="inlineStr">
         <is>
-          <t>VENTE MARCHAND</t>
+          <t>VENTE PARTICULIER</t>
         </is>
       </c>
       <c r="I14" s="0" t="inlineStr">
         <is>
-          <t>UU1B5220X63919206</t>
+          <t>VF1RJA00865717430</t>
         </is>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
       <c r="A15" s="0" t="n">
-        <v>80228</v>
+        <v>81408</v>
       </c>
       <c r="B15" s="0" t="inlineStr">
         <is>
-          <t>FF766BX</t>
+          <t>FX851NP</t>
         </is>
       </c>
       <c r="C15" s="0" t="inlineStr">
         <is>
-          <t>DALLARD AUTOMBILES 64</t>
+          <t>SABINE MOSER</t>
         </is>
       </c>
       <c r="D15" s="0" t="n">
-        <v>12166.67</v>
+        <v>11583.33</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>14600.00</v>
+        <v>13900.00</v>
       </c>
       <c r="F15" s="0" t="inlineStr">
         <is>
-          <t>YOHAN DUPONT </t>
+          <t>TOM FERRAGU </t>
         </is>
       </c>
       <c r="G15" s="0" t="inlineStr">
         <is>
-          <t>2023/06/14</t>
+          <t>2023/10/11</t>
         </is>
       </c>
       <c r="H15" s="0" t="inlineStr">
         <is>
-          <t>VENTE MARCHAND</t>
+          <t>VENTE PARTICULIER</t>
         </is>
       </c>
       <c r="I15" s="0" t="inlineStr">
         <is>
-          <t>VF3LBYHZPKS160345</t>
+          <t>VF1RFB00867111234</t>
         </is>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
       <c r="A16" s="0" t="n">
-        <v>80229</v>
+        <v>81411</v>
       </c>
       <c r="B16" s="0" t="inlineStr">
         <is>
-          <t>GB757BE</t>
+          <t>GK956EK</t>
         </is>
       </c>
       <c r="C16" s="0" t="inlineStr">
         <is>
-          <t>garage brut</t>
+          <t>ROMUALD TRIFFAULT</t>
         </is>
       </c>
       <c r="D16" s="0" t="n">
-        <v>12666.67</v>
+        <v>17900.00</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>15200.00</v>
+        <v>17900.00</v>
       </c>
       <c r="F16" s="0" t="inlineStr">
         <is>
-          <t>CLEMENT SAUSSET </t>
+          <t>FAYCAL BENHAMMOU </t>
         </is>
       </c>
       <c r="G16" s="0" t="inlineStr">
         <is>
-          <t>2023/06/14</t>
+          <t>2023/10/11</t>
         </is>
       </c>
       <c r="H16" s="0" t="inlineStr">
         <is>
-          <t>VENTE MARCHAND</t>
+          <t>VENTE PARTICULIER</t>
         </is>
       </c>
       <c r="I16" s="0" t="inlineStr">
         <is>
-          <t>VF1RJB00867931943</t>
+          <t>VF1RFB00856737533</t>
         </is>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
       <c r="A17" s="0" t="n">
-        <v>80229</v>
+        <v>81409</v>
       </c>
       <c r="B17" s="0" t="inlineStr">
         <is>
-          <t>FV760VR</t>
+          <t>FY964DF</t>
         </is>
       </c>
       <c r="C17" s="0" t="inlineStr">
         <is>
-          <t>garage brut</t>
+          <t>bernard fournier</t>
         </is>
       </c>
       <c r="D17" s="0" t="n">
-        <v>12083.33</v>
+        <v>12416.67</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>14500.00</v>
+        <v>14900.00</v>
       </c>
       <c r="F17" s="0" t="inlineStr">
         <is>
-          <t>CLEMENT SAUSSET </t>
+          <t>Patrice QUIET </t>
         </is>
       </c>
       <c r="G17" s="0" t="inlineStr">
         <is>
-          <t>2023/06/14</t>
+          <t>2023/10/11</t>
         </is>
       </c>
       <c r="H17" s="0" t="inlineStr">
         <is>
-          <t>VENTE MARCHAND</t>
+          <t>VENTE PARTICULIER</t>
         </is>
       </c>
       <c r="I17" s="0" t="inlineStr">
         <is>
-          <t>VF1RJA00066718808</t>
+          <t>W0VZRHNS2KS201580</t>
         </is>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
       <c r="A18" s="0" t="n">
-        <v>80230</v>
+        <v>81410</v>
       </c>
       <c r="B18" s="0" t="inlineStr">
         <is>
-          <t>FJ541VR</t>
+          <t>EW699GE</t>
         </is>
       </c>
       <c r="C18" s="0" t="inlineStr">
         <is>
-          <t>garage Delamare</t>
+          <t>BCAUTO ENCHERES</t>
         </is>
       </c>
       <c r="D18" s="0" t="n">
-        <v>8250.00</v>
+        <v>11583.33</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>9900.00</v>
+        <v>13900.00</v>
       </c>
       <c r="F18" s="0" t="inlineStr">
         <is>
-          <t>HUMBERTO ALVES </t>
+          <t>GUILLAUME HONNERT </t>
         </is>
       </c>
       <c r="G18" s="0" t="inlineStr">
         <is>
-          <t>2023/06/14</t>
+          <t>2023/10/11</t>
         </is>
       </c>
       <c r="H18" s="0" t="inlineStr">
@@ -857,48 +857,786 @@
       </c>
       <c r="I18" s="0" t="inlineStr">
         <is>
-          <t>VF1R9800X63001819</t>
+          <t>WF0DXXTTGDJL89071</t>
         </is>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
       <c r="A19" s="0" t="n">
-        <v>80231</v>
+        <v>81412</v>
       </c>
       <c r="B19" s="0" t="inlineStr">
         <is>
-          <t>FR984QB</t>
+          <t>FE243TY</t>
         </is>
       </c>
       <c r="C19" s="0" t="inlineStr">
         <is>
-          <t>SARL INTER VO FRANCE</t>
+          <t>Ben Ali CISSE</t>
         </is>
       </c>
       <c r="D19" s="0" t="n">
-        <v>10750.00</v>
+        <v>13666.67</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>12900.00</v>
+        <v>16400.00</v>
       </c>
       <c r="F19" s="0" t="inlineStr">
         <is>
-          <t>GUILLAUME HONNERT </t>
+          <t>MOSSO MAMET </t>
         </is>
       </c>
       <c r="G19" s="0" t="inlineStr">
         <is>
-          <t>2023/06/14</t>
+          <t>2023/10/11</t>
         </is>
       </c>
       <c r="H19" s="0" t="inlineStr">
         <is>
-          <t>VENTE MARCHAND</t>
+          <t>VENTE PARTICULIER</t>
         </is>
       </c>
       <c r="I19" s="0" t="inlineStr">
         <is>
-          <t>VF1RFB00765682306</t>
+          <t>VF1FL000462506945</t>
+        </is>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
+      <c r="A20" s="0" t="n">
+        <v>81413</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>GA657LK</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>SN DEPUSSAY</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>11583.33</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>13900.00</v>
+      </c>
+      <c r="F20" s="0" t="inlineStr">
+        <is>
+          <t>MOSSO MAMET </t>
+        </is>
+      </c>
+      <c r="G20" s="0" t="inlineStr">
+        <is>
+          <t>2023/10/11</t>
+        </is>
+      </c>
+      <c r="H20" s="0" t="inlineStr">
+        <is>
+          <t>VENTE PARTICULIER</t>
+        </is>
+      </c>
+      <c r="I20" s="0" t="inlineStr">
+        <is>
+          <t>VSSZZZ5FZLR096239</t>
+        </is>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
+      <c r="A21" s="0" t="n">
+        <v>81414</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>FL868BS</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>ACHATS GROUPE PELLEAU</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>8577.50</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>10293.00</v>
+      </c>
+      <c r="F21" s="0" t="inlineStr">
+        <is>
+          <t>GUILLAUME HONNERT </t>
+        </is>
+      </c>
+      <c r="G21" s="0" t="inlineStr">
+        <is>
+          <t>2023/10/11</t>
+        </is>
+      </c>
+      <c r="H21" s="0" t="inlineStr">
+        <is>
+          <t>VENTE MARCHAND</t>
+        </is>
+      </c>
+      <c r="I21" s="0" t="inlineStr">
+        <is>
+          <t>VF1R8700663587271</t>
+        </is>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
+      <c r="A22" s="0" t="n">
+        <v>81414</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>FE643JG</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>ACHATS GROUPE PELLEAU</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>7660.83</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>9193.00</v>
+      </c>
+      <c r="F22" s="0" t="inlineStr">
+        <is>
+          <t>GUILLAUME HONNERT </t>
+        </is>
+      </c>
+      <c r="G22" s="0" t="inlineStr">
+        <is>
+          <t>2023/10/11</t>
+        </is>
+      </c>
+      <c r="H22" s="0" t="inlineStr">
+        <is>
+          <t>VENTE MARCHAND</t>
+        </is>
+      </c>
+      <c r="I22" s="0" t="inlineStr">
+        <is>
+          <t>VF1R9800661894745</t>
+        </is>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
+      <c r="A23" s="0" t="n">
+        <v>81414</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>FD971RT</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>ACHATS GROUPE PELLEAU</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>4744.17</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>5693.00</v>
+      </c>
+      <c r="F23" s="0" t="inlineStr">
+        <is>
+          <t>GUILLAUME HONNERT </t>
+        </is>
+      </c>
+      <c r="G23" s="0" t="inlineStr">
+        <is>
+          <t>2023/10/11</t>
+        </is>
+      </c>
+      <c r="H23" s="0" t="inlineStr">
+        <is>
+          <t>VENTE MARCHAND</t>
+        </is>
+      </c>
+      <c r="I23" s="0" t="inlineStr">
+        <is>
+          <t>VF1R9800061851566</t>
+        </is>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
+      <c r="A24" s="0" t="n">
+        <v>81414</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>FQ587XT</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>ACHATS GROUPE PELLEAU</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>7744.17</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>9293.00</v>
+      </c>
+      <c r="F24" s="0" t="inlineStr">
+        <is>
+          <t>GUILLAUME HONNERT </t>
+        </is>
+      </c>
+      <c r="G24" s="0" t="inlineStr">
+        <is>
+          <t>2023/10/11</t>
+        </is>
+      </c>
+      <c r="H24" s="0" t="inlineStr">
+        <is>
+          <t>VENTE MARCHAND</t>
+        </is>
+      </c>
+      <c r="I24" s="0" t="inlineStr">
+        <is>
+          <t>VF1RJA00065895798</t>
+        </is>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
+      <c r="A25" s="0" t="n">
+        <v>81414</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>FT073TQ</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>ACHATS GROUPE PELLEAU</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>8160.83</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>9793.00</v>
+      </c>
+      <c r="F25" s="0" t="inlineStr">
+        <is>
+          <t>GUILLAUME HONNERT </t>
+        </is>
+      </c>
+      <c r="G25" s="0" t="inlineStr">
+        <is>
+          <t>2023/10/11</t>
+        </is>
+      </c>
+      <c r="H25" s="0" t="inlineStr">
+        <is>
+          <t>VENTE MARCHAND</t>
+        </is>
+      </c>
+      <c r="I25" s="0" t="inlineStr">
+        <is>
+          <t>VF1RJA00166194455</t>
+        </is>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
+      <c r="A26" s="0" t="n">
+        <v>81414</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>GB104WM</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>ACHATS GROUPE PELLEAU</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>12660.83</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>15193.00</v>
+      </c>
+      <c r="F26" s="0" t="inlineStr">
+        <is>
+          <t>GUILLAUME HONNERT </t>
+        </is>
+      </c>
+      <c r="G26" s="0" t="inlineStr">
+        <is>
+          <t>2023/10/11</t>
+        </is>
+      </c>
+      <c r="H26" s="0" t="inlineStr">
+        <is>
+          <t>VENTE MARCHAND</t>
+        </is>
+      </c>
+      <c r="I26" s="0" t="inlineStr">
+        <is>
+          <t>VF1RFE00868106790</t>
+        </is>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27">
+      <c r="A27" s="0" t="n">
+        <v>81414</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>FN446QN</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>ACHATS GROUPE PELLEAU</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>8910.83</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>10693.00</v>
+      </c>
+      <c r="F27" s="0" t="inlineStr">
+        <is>
+          <t>GUILLAUME HONNERT </t>
+        </is>
+      </c>
+      <c r="G27" s="0" t="inlineStr">
+        <is>
+          <t>2023/10/11</t>
+        </is>
+      </c>
+      <c r="H27" s="0" t="inlineStr">
+        <is>
+          <t>VENTE MARCHAND</t>
+        </is>
+      </c>
+      <c r="I27" s="0" t="inlineStr">
+        <is>
+          <t>VF1RFB00165056508</t>
+        </is>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
+      <c r="A28" s="0" t="n">
+        <v>81414</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>FH545LZ</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>ACHATS GROUPE PELLEAU</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>8910.83</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>10693.00</v>
+      </c>
+      <c r="F28" s="0" t="inlineStr">
+        <is>
+          <t>GUILLAUME HONNERT </t>
+        </is>
+      </c>
+      <c r="G28" s="0" t="inlineStr">
+        <is>
+          <t>2023/10/11</t>
+        </is>
+      </c>
+      <c r="H28" s="0" t="inlineStr">
+        <is>
+          <t>VENTE MARCHAND</t>
+        </is>
+      </c>
+      <c r="I28" s="0" t="inlineStr">
+        <is>
+          <t>VF1RFB00963486475</t>
+        </is>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
+      <c r="A29" s="0" t="n">
+        <v>81414</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>FD824HM</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>ACHATS GROUPE PELLEAU</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>9827.50</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>11793.00</v>
+      </c>
+      <c r="F29" s="0" t="inlineStr">
+        <is>
+          <t>GUILLAUME HONNERT </t>
+        </is>
+      </c>
+      <c r="G29" s="0" t="inlineStr">
+        <is>
+          <t>2023/10/11</t>
+        </is>
+      </c>
+      <c r="H29" s="0" t="inlineStr">
+        <is>
+          <t>VENTE MARCHAND</t>
+        </is>
+      </c>
+      <c r="I29" s="0" t="inlineStr">
+        <is>
+          <t>VF1RFB00061205756</t>
+        </is>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
+      <c r="A30" s="0" t="n">
+        <v>81414</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>FQ220XV</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>ACHATS GROUPE PELLEAU</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>9910.83</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>11893.00</v>
+      </c>
+      <c r="F30" s="0" t="inlineStr">
+        <is>
+          <t>GUILLAUME HONNERT </t>
+        </is>
+      </c>
+      <c r="G30" s="0" t="inlineStr">
+        <is>
+          <t>2023/10/11</t>
+        </is>
+      </c>
+      <c r="H30" s="0" t="inlineStr">
+        <is>
+          <t>VENTE MARCHAND</t>
+        </is>
+      </c>
+      <c r="I30" s="0" t="inlineStr">
+        <is>
+          <t>VF1RFB00165705787</t>
+        </is>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="31">
+      <c r="A31" s="0" t="n">
+        <v>81414</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>FV820QY</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>ACHATS GROUPE PELLEAU</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>7660.83</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>9193.00</v>
+      </c>
+      <c r="F31" s="0" t="inlineStr">
+        <is>
+          <t>GUILLAUME HONNERT </t>
+        </is>
+      </c>
+      <c r="G31" s="0" t="inlineStr">
+        <is>
+          <t>2023/10/11</t>
+        </is>
+      </c>
+      <c r="H31" s="0" t="inlineStr">
+        <is>
+          <t>VENTE MARCHAND</t>
+        </is>
+      </c>
+      <c r="I31" s="0" t="inlineStr">
+        <is>
+          <t>UU1DBG000LU002718</t>
+        </is>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32">
+      <c r="A32" s="0" t="n">
+        <v>81414</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>FY162HZ</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>ACHATS GROUPE PELLEAU</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>7744.17</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>9293.00</v>
+      </c>
+      <c r="F32" s="0" t="inlineStr">
+        <is>
+          <t>GUILLAUME HONNERT </t>
+        </is>
+      </c>
+      <c r="G32" s="0" t="inlineStr">
+        <is>
+          <t>2023/10/11</t>
+        </is>
+      </c>
+      <c r="H32" s="0" t="inlineStr">
+        <is>
+          <t>VENTE MARCHAND</t>
+        </is>
+      </c>
+      <c r="I32" s="0" t="inlineStr">
+        <is>
+          <t>UU1DBG009LU004094</t>
+        </is>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="33">
+      <c r="A33" s="0" t="n">
+        <v>81414</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>FY967PB</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>ACHATS GROUPE PELLEAU</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>7994.17</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>9593.00</v>
+      </c>
+      <c r="F33" s="0" t="inlineStr">
+        <is>
+          <t>GUILLAUME HONNERT </t>
+        </is>
+      </c>
+      <c r="G33" s="0" t="inlineStr">
+        <is>
+          <t>2023/10/11</t>
+        </is>
+      </c>
+      <c r="H33" s="0" t="inlineStr">
+        <is>
+          <t>VENTE MARCHAND</t>
+        </is>
+      </c>
+      <c r="I33" s="0" t="inlineStr">
+        <is>
+          <t>UU1DBG003MU006084</t>
+        </is>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="34">
+      <c r="A34" s="0" t="n">
+        <v>81415</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>EY108CQ</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>GILLES GAYMARD</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>9991.67</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>11990.00</v>
+      </c>
+      <c r="F34" s="0" t="inlineStr">
+        <is>
+          <t>TOM FERRAGU </t>
+        </is>
+      </c>
+      <c r="G34" s="0" t="inlineStr">
+        <is>
+          <t>2023/10/11</t>
+        </is>
+      </c>
+      <c r="H34" s="0" t="inlineStr">
+        <is>
+          <t>VENTE PARTICULIER</t>
+        </is>
+      </c>
+      <c r="I34" s="0" t="inlineStr">
+        <is>
+          <t>UU15SDKJC60860468</t>
+        </is>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="35">
+      <c r="A35" s="0" t="n">
+        <v>81416</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>FQ442GY</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>Jose Luis MORENO</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>14083.33</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>16900.00</v>
+      </c>
+      <c r="F35" s="0" t="inlineStr">
+        <is>
+          <t>MOSSO MAMET </t>
+        </is>
+      </c>
+      <c r="G35" s="0" t="inlineStr">
+        <is>
+          <t>2023/10/11</t>
+        </is>
+      </c>
+      <c r="H35" s="0" t="inlineStr">
+        <is>
+          <t>VENTE PARTICULIER</t>
+        </is>
+      </c>
+      <c r="I35" s="0" t="inlineStr">
+        <is>
+          <t>VF1RFE00165166752</t>
+        </is>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="36">
+      <c r="A36" s="0" t="n">
+        <v>81417</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>FG905YQ</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>ALISON MAUCORPS</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>8250.00</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>9900.00</v>
+      </c>
+      <c r="F36" s="0" t="inlineStr">
+        <is>
+          <t>FAYCAL BENHAMMOU </t>
+        </is>
+      </c>
+      <c r="G36" s="0" t="inlineStr">
+        <is>
+          <t>2023/10/11</t>
+        </is>
+      </c>
+      <c r="H36" s="0" t="inlineStr">
+        <is>
+          <t>VENTE PARTICULIER</t>
+        </is>
+      </c>
+      <c r="I36" s="0" t="inlineStr">
+        <is>
+          <t>ZFA35600006N75312</t>
+        </is>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="37">
+      <c r="A37" s="0" t="n">
+        <v>81418</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>FS391XG</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>INTER V.O FRANCE</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>10416.67</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>12500.00</v>
+      </c>
+      <c r="F37" s="0" t="inlineStr">
+        <is>
+          <t>GUILLAUME HONNERT </t>
+        </is>
+      </c>
+      <c r="G37" s="0" t="inlineStr">
+        <is>
+          <t>2023/10/11</t>
+        </is>
+      </c>
+      <c r="H37" s="0" t="inlineStr">
+        <is>
+          <t>VENTE MARCHAND</t>
+        </is>
+      </c>
+      <c r="I37" s="0" t="inlineStr">
+        <is>
+          <t>VF1RFB00566134668</t>
         </is>
       </c>
     </row>

</xml_diff>